<commit_message>
input csv and general output pickle
</commit_message>
<xml_diff>
--- a/input/datasets.xlsx
+++ b/input/datasets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="alldata" sheetId="1" r:id="rId1"/>
@@ -2676,14 +2676,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R183"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P155" sqref="P155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9762,10 +9763,10 @@
         <v>486</v>
       </c>
       <c r="O152" t="s">
+        <v>281</v>
+      </c>
+      <c r="P152" t="s">
         <v>280</v>
-      </c>
-      <c r="P152" t="s">
-        <v>281</v>
       </c>
       <c r="Q152" t="s">
         <v>321</v>
@@ -9806,10 +9807,10 @@
         <v>486</v>
       </c>
       <c r="O153" t="s">
+        <v>281</v>
+      </c>
+      <c r="P153" t="s">
         <v>280</v>
-      </c>
-      <c r="P153" t="s">
-        <v>281</v>
       </c>
       <c r="Q153" t="s">
         <v>321</v>
@@ -9850,10 +9851,10 @@
         <v>486</v>
       </c>
       <c r="O154" t="s">
+        <v>281</v>
+      </c>
+      <c r="P154" t="s">
         <v>280</v>
-      </c>
-      <c r="P154" t="s">
-        <v>281</v>
       </c>
       <c r="Q154" t="s">
         <v>321</v>
@@ -9894,10 +9895,10 @@
         <v>486</v>
       </c>
       <c r="O155" t="s">
+        <v>281</v>
+      </c>
+      <c r="P155" t="s">
         <v>280</v>
-      </c>
-      <c r="P155" t="s">
-        <v>281</v>
       </c>
       <c r="Q155" t="s">
         <v>321</v>
@@ -9938,10 +9939,10 @@
         <v>486</v>
       </c>
       <c r="O156" t="s">
+        <v>281</v>
+      </c>
+      <c r="P156" t="s">
         <v>280</v>
-      </c>
-      <c r="P156" t="s">
-        <v>281</v>
       </c>
       <c r="Q156" t="s">
         <v>321</v>
@@ -9982,10 +9983,10 @@
         <v>486</v>
       </c>
       <c r="O157" t="s">
+        <v>281</v>
+      </c>
+      <c r="P157" t="s">
         <v>280</v>
-      </c>
-      <c r="P157" t="s">
-        <v>281</v>
       </c>
       <c r="Q157" t="s">
         <v>321</v>
@@ -10026,10 +10027,10 @@
         <v>486</v>
       </c>
       <c r="O158" t="s">
+        <v>281</v>
+      </c>
+      <c r="P158" t="s">
         <v>280</v>
-      </c>
-      <c r="P158" t="s">
-        <v>281</v>
       </c>
       <c r="Q158" t="s">
         <v>321</v>
@@ -10070,10 +10071,10 @@
         <v>486</v>
       </c>
       <c r="O159" t="s">
+        <v>281</v>
+      </c>
+      <c r="P159" t="s">
         <v>280</v>
-      </c>
-      <c r="P159" t="s">
-        <v>281</v>
       </c>
       <c r="Q159" t="s">
         <v>321</v>
@@ -10114,10 +10115,10 @@
         <v>486</v>
       </c>
       <c r="O160" t="s">
+        <v>281</v>
+      </c>
+      <c r="P160" t="s">
         <v>280</v>
-      </c>
-      <c r="P160" t="s">
-        <v>281</v>
       </c>
       <c r="Q160" t="s">
         <v>321</v>
@@ -10158,10 +10159,10 @@
         <v>486</v>
       </c>
       <c r="O161" t="s">
+        <v>281</v>
+      </c>
+      <c r="P161" t="s">
         <v>280</v>
-      </c>
-      <c r="P161" t="s">
-        <v>281</v>
       </c>
       <c r="Q161" t="s">
         <v>321</v>
@@ -10202,10 +10203,10 @@
         <v>486</v>
       </c>
       <c r="O162" t="s">
+        <v>281</v>
+      </c>
+      <c r="P162" t="s">
         <v>280</v>
-      </c>
-      <c r="P162" t="s">
-        <v>281</v>
       </c>
       <c r="Q162" t="s">
         <v>321</v>
@@ -10246,10 +10247,10 @@
         <v>486</v>
       </c>
       <c r="O163" t="s">
+        <v>281</v>
+      </c>
+      <c r="P163" t="s">
         <v>280</v>
-      </c>
-      <c r="P163" t="s">
-        <v>281</v>
       </c>
       <c r="Q163" t="s">
         <v>321</v>
@@ -10290,10 +10291,10 @@
         <v>486</v>
       </c>
       <c r="O164" t="s">
+        <v>281</v>
+      </c>
+      <c r="P164" t="s">
         <v>280</v>
-      </c>
-      <c r="P164" t="s">
-        <v>281</v>
       </c>
       <c r="Q164" t="s">
         <v>321</v>
@@ -10334,10 +10335,10 @@
         <v>486</v>
       </c>
       <c r="O165" t="s">
+        <v>281</v>
+      </c>
+      <c r="P165" t="s">
         <v>280</v>
-      </c>
-      <c r="P165" t="s">
-        <v>281</v>
       </c>
       <c r="Q165" t="s">
         <v>321</v>
@@ -10378,10 +10379,10 @@
         <v>486</v>
       </c>
       <c r="O166" t="s">
+        <v>281</v>
+      </c>
+      <c r="P166" t="s">
         <v>280</v>
-      </c>
-      <c r="P166" t="s">
-        <v>281</v>
       </c>
       <c r="Q166" t="s">
         <v>321</v>
@@ -10422,10 +10423,10 @@
         <v>486</v>
       </c>
       <c r="O167" t="s">
+        <v>281</v>
+      </c>
+      <c r="P167" t="s">
         <v>280</v>
-      </c>
-      <c r="P167" t="s">
-        <v>281</v>
       </c>
       <c r="Q167" t="s">
         <v>321</v>
@@ -10466,10 +10467,10 @@
         <v>486</v>
       </c>
       <c r="O168" t="s">
+        <v>281</v>
+      </c>
+      <c r="P168" t="s">
         <v>280</v>
-      </c>
-      <c r="P168" t="s">
-        <v>281</v>
       </c>
       <c r="Q168" t="s">
         <v>321</v>
@@ -10510,10 +10511,10 @@
         <v>486</v>
       </c>
       <c r="O169" t="s">
+        <v>281</v>
+      </c>
+      <c r="P169" t="s">
         <v>280</v>
-      </c>
-      <c r="P169" t="s">
-        <v>281</v>
       </c>
       <c r="Q169" t="s">
         <v>321</v>
@@ -10554,10 +10555,10 @@
         <v>486</v>
       </c>
       <c r="O170" t="s">
+        <v>281</v>
+      </c>
+      <c r="P170" t="s">
         <v>280</v>
-      </c>
-      <c r="P170" t="s">
-        <v>281</v>
       </c>
       <c r="Q170" t="s">
         <v>321</v>
@@ -10598,10 +10599,10 @@
         <v>486</v>
       </c>
       <c r="O171" t="s">
+        <v>281</v>
+      </c>
+      <c r="P171" t="s">
         <v>280</v>
-      </c>
-      <c r="P171" t="s">
-        <v>281</v>
       </c>
       <c r="Q171" t="s">
         <v>321</v>
@@ -10642,10 +10643,10 @@
         <v>486</v>
       </c>
       <c r="O172" t="s">
+        <v>281</v>
+      </c>
+      <c r="P172" t="s">
         <v>280</v>
-      </c>
-      <c r="P172" t="s">
-        <v>281</v>
       </c>
       <c r="Q172" t="s">
         <v>321</v>
@@ -10686,10 +10687,10 @@
         <v>486</v>
       </c>
       <c r="O173" t="s">
+        <v>281</v>
+      </c>
+      <c r="P173" t="s">
         <v>280</v>
-      </c>
-      <c r="P173" t="s">
-        <v>281</v>
       </c>
       <c r="Q173" t="s">
         <v>321</v>
@@ -10730,10 +10731,10 @@
         <v>486</v>
       </c>
       <c r="O174" t="s">
+        <v>281</v>
+      </c>
+      <c r="P174" t="s">
         <v>280</v>
-      </c>
-      <c r="P174" t="s">
-        <v>281</v>
       </c>
       <c r="Q174" t="s">
         <v>321</v>
@@ -10774,10 +10775,10 @@
         <v>486</v>
       </c>
       <c r="O175" t="s">
+        <v>281</v>
+      </c>
+      <c r="P175" t="s">
         <v>280</v>
-      </c>
-      <c r="P175" t="s">
-        <v>281</v>
       </c>
       <c r="Q175" t="s">
         <v>321</v>
@@ -10818,10 +10819,10 @@
         <v>486</v>
       </c>
       <c r="O176" t="s">
+        <v>281</v>
+      </c>
+      <c r="P176" t="s">
         <v>280</v>
-      </c>
-      <c r="P176" t="s">
-        <v>281</v>
       </c>
       <c r="Q176" t="s">
         <v>321</v>
@@ -10862,10 +10863,10 @@
         <v>486</v>
       </c>
       <c r="O177" t="s">
+        <v>281</v>
+      </c>
+      <c r="P177" t="s">
         <v>280</v>
-      </c>
-      <c r="P177" t="s">
-        <v>281</v>
       </c>
       <c r="Q177" t="s">
         <v>321</v>
@@ -10906,10 +10907,10 @@
         <v>486</v>
       </c>
       <c r="O178" t="s">
+        <v>281</v>
+      </c>
+      <c r="P178" t="s">
         <v>280</v>
-      </c>
-      <c r="P178" t="s">
-        <v>281</v>
       </c>
       <c r="Q178" t="s">
         <v>321</v>
@@ -10950,10 +10951,10 @@
         <v>486</v>
       </c>
       <c r="O179" t="s">
+        <v>281</v>
+      </c>
+      <c r="P179" t="s">
         <v>280</v>
-      </c>
-      <c r="P179" t="s">
-        <v>281</v>
       </c>
       <c r="Q179" t="s">
         <v>321</v>
@@ -10994,10 +10995,10 @@
         <v>486</v>
       </c>
       <c r="O180" t="s">
+        <v>281</v>
+      </c>
+      <c r="P180" t="s">
         <v>280</v>
-      </c>
-      <c r="P180" t="s">
-        <v>281</v>
       </c>
       <c r="Q180" t="s">
         <v>321</v>
@@ -11038,10 +11039,10 @@
         <v>486</v>
       </c>
       <c r="O181" t="s">
+        <v>281</v>
+      </c>
+      <c r="P181" t="s">
         <v>280</v>
-      </c>
-      <c r="P181" t="s">
-        <v>281</v>
       </c>
       <c r="Q181" t="s">
         <v>321</v>
@@ -11082,10 +11083,10 @@
         <v>486</v>
       </c>
       <c r="O182" t="s">
+        <v>281</v>
+      </c>
+      <c r="P182" t="s">
         <v>280</v>
-      </c>
-      <c r="P182" t="s">
-        <v>281</v>
       </c>
       <c r="Q182" t="s">
         <v>321</v>
@@ -11126,10 +11127,10 @@
         <v>486</v>
       </c>
       <c r="O183" t="s">
+        <v>281</v>
+      </c>
+      <c r="P183" t="s">
         <v>280</v>
-      </c>
-      <c r="P183" t="s">
-        <v>281</v>
       </c>
       <c r="Q183" t="s">
         <v>321</v>
@@ -13391,8 +13392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
alternative postfix sequences for better read finding
</commit_message>
<xml_diff>
--- a/input/datasets.xlsx
+++ b/input/datasets.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="507">
   <si>
     <t>date_sequenced</t>
   </si>
@@ -1525,6 +1525,27 @@
   </si>
   <si>
     <t>5,[sal1,atc,cin]</t>
+  </si>
+  <si>
+    <t>GCAGGGCGGTTTTTCGAAGGTTCTCTGAGCTACCAACTCTTTGAACCG</t>
+  </si>
+  <si>
+    <t>i57_chunk</t>
+  </si>
+  <si>
+    <t>u21attb</t>
+  </si>
+  <si>
+    <t>u22attb</t>
+  </si>
+  <si>
+    <t>TCCGTCTACGAACTCCCAGCAGGTAGGTATGATCCTGACGACGGAGCACGCCGTCGTCGACAAGCC</t>
+  </si>
+  <si>
+    <t>GCTTGGATTCTGCGTTTGTTAGGTATGATCCTGACGACGGAGCACGCCGTCGTCGACAAGCC</t>
+  </si>
+  <si>
+    <t>[genomechunk,i57_chunk]</t>
   </si>
 </sst>
 </file>
@@ -2677,8 +2698,8 @@
   <dimension ref="A1:R183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P155" sqref="P155"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W129" sqref="W129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,7 +2990,7 @@
         <v>43412</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O10" t="s">
         <v>277</v>
@@ -3022,7 +3043,7 @@
         <v>43412</v>
       </c>
       <c r="N11" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O11" t="s">
         <v>277</v>
@@ -3075,7 +3096,7 @@
         <v>43412</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O12" t="s">
         <v>277</v>
@@ -3128,7 +3149,7 @@
         <v>43412</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O13" t="s">
         <v>277</v>
@@ -3181,7 +3202,7 @@
         <v>43412</v>
       </c>
       <c r="N14" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O14" t="s">
         <v>277</v>
@@ -3234,7 +3255,7 @@
         <v>43412</v>
       </c>
       <c r="N15" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O15" t="s">
         <v>277</v>
@@ -3287,7 +3308,7 @@
         <v>43412</v>
       </c>
       <c r="N16" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O16" t="s">
         <v>277</v>
@@ -3340,7 +3361,7 @@
         <v>43412</v>
       </c>
       <c r="N17" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O17" t="s">
         <v>277</v>
@@ -3393,7 +3414,7 @@
         <v>43412</v>
       </c>
       <c r="N18" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O18" t="s">
         <v>277</v>
@@ -3446,7 +3467,7 @@
         <v>43412</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O19" t="s">
         <v>277</v>
@@ -3499,7 +3520,7 @@
         <v>43418</v>
       </c>
       <c r="N20" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O20" t="s">
         <v>277</v>
@@ -3552,7 +3573,7 @@
         <v>43418</v>
       </c>
       <c r="N21" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O21" t="s">
         <v>277</v>
@@ -3605,7 +3626,7 @@
         <v>43418</v>
       </c>
       <c r="N22" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O22" t="s">
         <v>277</v>
@@ -3658,7 +3679,7 @@
         <v>43418</v>
       </c>
       <c r="N23" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O23" t="s">
         <v>277</v>
@@ -3711,7 +3732,7 @@
         <v>43418</v>
       </c>
       <c r="N24" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O24" t="s">
         <v>277</v>
@@ -3764,7 +3785,7 @@
         <v>43418</v>
       </c>
       <c r="N25" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O25" t="s">
         <v>277</v>
@@ -3817,7 +3838,7 @@
         <v>43418</v>
       </c>
       <c r="N26" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O26" t="s">
         <v>277</v>
@@ -3870,7 +3891,7 @@
         <v>43418</v>
       </c>
       <c r="N27" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O27" t="s">
         <v>277</v>
@@ -3923,7 +3944,7 @@
         <v>43418</v>
       </c>
       <c r="N28" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O28" t="s">
         <v>277</v>
@@ -3976,7 +3997,7 @@
         <v>43418</v>
       </c>
       <c r="N29" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O29" t="s">
         <v>277</v>
@@ -4023,7 +4044,7 @@
         <v>43479</v>
       </c>
       <c r="N30" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O30" t="s">
         <v>277</v>
@@ -4070,7 +4091,7 @@
         <v>43479</v>
       </c>
       <c r="N31" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O31" t="s">
         <v>277</v>
@@ -4117,7 +4138,7 @@
         <v>43479</v>
       </c>
       <c r="N32" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O32" t="s">
         <v>277</v>
@@ -4164,7 +4185,7 @@
         <v>43479</v>
       </c>
       <c r="N33" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O33" t="s">
         <v>277</v>
@@ -4211,7 +4232,7 @@
         <v>43479</v>
       </c>
       <c r="N34" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O34" t="s">
         <v>277</v>
@@ -4258,7 +4279,7 @@
         <v>43479</v>
       </c>
       <c r="N35" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O35" t="s">
         <v>277</v>
@@ -4305,7 +4326,7 @@
         <v>43479</v>
       </c>
       <c r="N36" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O36" t="s">
         <v>277</v>
@@ -4352,7 +4373,7 @@
         <v>43479</v>
       </c>
       <c r="N37" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O37" t="s">
         <v>277</v>
@@ -4399,7 +4420,7 @@
         <v>43479</v>
       </c>
       <c r="N38" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O38" t="s">
         <v>277</v>
@@ -4446,7 +4467,7 @@
         <v>43479</v>
       </c>
       <c r="N39" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O39" t="s">
         <v>277</v>
@@ -4493,7 +4514,7 @@
         <v>43479</v>
       </c>
       <c r="N40" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O40" t="s">
         <v>277</v>
@@ -4540,7 +4561,7 @@
         <v>43479</v>
       </c>
       <c r="N41" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O41" t="s">
         <v>277</v>
@@ -4590,7 +4611,7 @@
         <v>43496</v>
       </c>
       <c r="N42" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O42" t="s">
         <v>277</v>
@@ -4640,7 +4661,7 @@
         <v>43496</v>
       </c>
       <c r="N43" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O43" t="s">
         <v>277</v>
@@ -4690,7 +4711,7 @@
         <v>43496</v>
       </c>
       <c r="N44" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O44" t="s">
         <v>277</v>
@@ -4740,7 +4761,7 @@
         <v>43496</v>
       </c>
       <c r="N45" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O45" t="s">
         <v>277</v>
@@ -4790,7 +4811,7 @@
         <v>43496</v>
       </c>
       <c r="N46" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O46" t="s">
         <v>277</v>
@@ -4840,7 +4861,7 @@
         <v>43496</v>
       </c>
       <c r="N47" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O47" t="s">
         <v>277</v>
@@ -4890,7 +4911,7 @@
         <v>43496</v>
       </c>
       <c r="N48" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O48" t="s">
         <v>277</v>
@@ -4940,7 +4961,7 @@
         <v>43496</v>
       </c>
       <c r="N49" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O49" t="s">
         <v>277</v>
@@ -4990,7 +5011,7 @@
         <v>43496</v>
       </c>
       <c r="N50" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O50" t="s">
         <v>277</v>
@@ -5040,7 +5061,7 @@
         <v>43496</v>
       </c>
       <c r="N51" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O51" t="s">
         <v>277</v>
@@ -5090,7 +5111,7 @@
         <v>43496</v>
       </c>
       <c r="N52" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O52" t="s">
         <v>277</v>
@@ -5140,7 +5161,7 @@
         <v>43496</v>
       </c>
       <c r="N53" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O53" t="s">
         <v>277</v>
@@ -5190,7 +5211,7 @@
         <v>43496</v>
       </c>
       <c r="N54" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O54" t="s">
         <v>277</v>
@@ -5240,7 +5261,7 @@
         <v>43496</v>
       </c>
       <c r="N55" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O55" t="s">
         <v>277</v>
@@ -5290,7 +5311,7 @@
         <v>43496</v>
       </c>
       <c r="N56" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O56" t="s">
         <v>277</v>
@@ -5340,7 +5361,7 @@
         <v>43515</v>
       </c>
       <c r="N57" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O57" t="s">
         <v>277</v>
@@ -5349,7 +5370,7 @@
         <v>276</v>
       </c>
       <c r="Q57" t="s">
-        <v>321</v>
+        <v>501</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -5390,7 +5411,7 @@
         <v>43515</v>
       </c>
       <c r="N58" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O58" t="s">
         <v>277</v>
@@ -5399,7 +5420,7 @@
         <v>276</v>
       </c>
       <c r="Q58" t="s">
-        <v>321</v>
+        <v>501</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
@@ -5440,7 +5461,7 @@
         <v>43515</v>
       </c>
       <c r="N59" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O59" t="s">
         <v>277</v>
@@ -5449,7 +5470,7 @@
         <v>276</v>
       </c>
       <c r="Q59" t="s">
-        <v>321</v>
+        <v>501</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -5490,7 +5511,7 @@
         <v>43515</v>
       </c>
       <c r="N60" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O60" t="s">
         <v>277</v>
@@ -5499,7 +5520,7 @@
         <v>276</v>
       </c>
       <c r="Q60" t="s">
-        <v>321</v>
+        <v>501</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -5540,7 +5561,7 @@
         <v>43515</v>
       </c>
       <c r="N61" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O61" t="s">
         <v>277</v>
@@ -5549,7 +5570,7 @@
         <v>276</v>
       </c>
       <c r="Q61" t="s">
-        <v>321</v>
+        <v>501</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -5590,7 +5611,7 @@
         <v>43515</v>
       </c>
       <c r="N62" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O62" t="s">
         <v>277</v>
@@ -5599,7 +5620,7 @@
         <v>276</v>
       </c>
       <c r="Q62" t="s">
-        <v>321</v>
+        <v>501</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -5640,7 +5661,7 @@
         <v>43515</v>
       </c>
       <c r="N63" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O63" t="s">
         <v>277</v>
@@ -5649,7 +5670,7 @@
         <v>276</v>
       </c>
       <c r="Q63" t="s">
-        <v>321</v>
+        <v>501</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -5690,7 +5711,7 @@
         <v>43515</v>
       </c>
       <c r="N64" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O64" t="s">
         <v>277</v>
@@ -5699,7 +5720,7 @@
         <v>276</v>
       </c>
       <c r="Q64" t="s">
-        <v>321</v>
+        <v>501</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
@@ -5740,7 +5761,7 @@
         <v>43515</v>
       </c>
       <c r="N65" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O65" t="s">
         <v>277</v>
@@ -5749,7 +5770,7 @@
         <v>276</v>
       </c>
       <c r="Q65" t="s">
-        <v>321</v>
+        <v>501</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -5793,7 +5814,7 @@
         <v>43523</v>
       </c>
       <c r="N66" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O66" t="s">
         <v>277</v>
@@ -5846,7 +5867,7 @@
         <v>43523</v>
       </c>
       <c r="N67" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O67" t="s">
         <v>277</v>
@@ -5899,7 +5920,7 @@
         <v>43523</v>
       </c>
       <c r="N68" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O68" t="s">
         <v>277</v>
@@ -5952,7 +5973,7 @@
         <v>43523</v>
       </c>
       <c r="N69" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O69" t="s">
         <v>277</v>
@@ -6005,7 +6026,7 @@
         <v>43523</v>
       </c>
       <c r="N70" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O70" t="s">
         <v>277</v>
@@ -6058,7 +6079,7 @@
         <v>43523</v>
       </c>
       <c r="N71" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O71" t="s">
         <v>277</v>
@@ -6111,7 +6132,7 @@
         <v>43523</v>
       </c>
       <c r="N72" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O72" t="s">
         <v>277</v>
@@ -6164,7 +6185,7 @@
         <v>43523</v>
       </c>
       <c r="N73" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O73" t="s">
         <v>277</v>
@@ -6217,7 +6238,7 @@
         <v>43523</v>
       </c>
       <c r="N74" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O74" t="s">
         <v>277</v>
@@ -6270,7 +6291,7 @@
         <v>43531</v>
       </c>
       <c r="N75" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O75" t="s">
         <v>277</v>
@@ -6279,7 +6300,7 @@
         <v>276</v>
       </c>
       <c r="Q75" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
@@ -6323,7 +6344,7 @@
         <v>43531</v>
       </c>
       <c r="N76" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O76" t="s">
         <v>277</v>
@@ -6332,7 +6353,7 @@
         <v>276</v>
       </c>
       <c r="Q76" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
@@ -6376,7 +6397,7 @@
         <v>43531</v>
       </c>
       <c r="N77" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O77" t="s">
         <v>277</v>
@@ -6385,7 +6406,7 @@
         <v>276</v>
       </c>
       <c r="Q77" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
@@ -6429,7 +6450,7 @@
         <v>43531</v>
       </c>
       <c r="N78" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O78" t="s">
         <v>277</v>
@@ -6438,7 +6459,7 @@
         <v>276</v>
       </c>
       <c r="Q78" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
@@ -6482,7 +6503,7 @@
         <v>43531</v>
       </c>
       <c r="N79" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O79" t="s">
         <v>277</v>
@@ -6491,7 +6512,7 @@
         <v>276</v>
       </c>
       <c r="Q79" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
@@ -6535,7 +6556,7 @@
         <v>43531</v>
       </c>
       <c r="N80" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O80" t="s">
         <v>277</v>
@@ -6544,7 +6565,7 @@
         <v>276</v>
       </c>
       <c r="Q80" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
@@ -6588,7 +6609,7 @@
         <v>43531</v>
       </c>
       <c r="N81" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O81" t="s">
         <v>277</v>
@@ -6597,7 +6618,7 @@
         <v>276</v>
       </c>
       <c r="Q81" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
@@ -6641,7 +6662,7 @@
         <v>43531</v>
       </c>
       <c r="N82" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O82" t="s">
         <v>277</v>
@@ -6650,7 +6671,7 @@
         <v>276</v>
       </c>
       <c r="Q82" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
@@ -6694,7 +6715,7 @@
         <v>43531</v>
       </c>
       <c r="N83" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O83" t="s">
         <v>277</v>
@@ -6703,7 +6724,7 @@
         <v>276</v>
       </c>
       <c r="Q83" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
@@ -6747,7 +6768,7 @@
         <v>43531</v>
       </c>
       <c r="N84" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O84" t="s">
         <v>277</v>
@@ -6756,7 +6777,7 @@
         <v>276</v>
       </c>
       <c r="Q84" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
@@ -6800,7 +6821,7 @@
         <v>43531</v>
       </c>
       <c r="N85" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O85" t="s">
         <v>277</v>
@@ -6809,7 +6830,7 @@
         <v>276</v>
       </c>
       <c r="Q85" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
@@ -6853,7 +6874,7 @@
         <v>43531</v>
       </c>
       <c r="N86" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O86" t="s">
         <v>277</v>
@@ -6862,7 +6883,7 @@
         <v>276</v>
       </c>
       <c r="Q86" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
@@ -6906,7 +6927,7 @@
         <v>43531</v>
       </c>
       <c r="N87" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O87" t="s">
         <v>277</v>
@@ -6915,7 +6936,7 @@
         <v>276</v>
       </c>
       <c r="Q87" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
@@ -6959,7 +6980,7 @@
         <v>43531</v>
       </c>
       <c r="N88" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O88" t="s">
         <v>277</v>
@@ -6968,7 +6989,7 @@
         <v>276</v>
       </c>
       <c r="Q88" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
@@ -7012,7 +7033,7 @@
         <v>43531</v>
       </c>
       <c r="N89" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O89" t="s">
         <v>277</v>
@@ -7021,7 +7042,7 @@
         <v>276</v>
       </c>
       <c r="Q89" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
@@ -7056,7 +7077,7 @@
         <v>333</v>
       </c>
       <c r="N90" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O90" t="s">
         <v>277</v>
@@ -7065,7 +7086,7 @@
         <v>276</v>
       </c>
       <c r="Q90" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
@@ -7100,7 +7121,7 @@
         <v>335</v>
       </c>
       <c r="N91" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O91" t="s">
         <v>277</v>
@@ -7109,7 +7130,7 @@
         <v>276</v>
       </c>
       <c r="Q91" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
@@ -7144,7 +7165,7 @@
         <v>336</v>
       </c>
       <c r="N92" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O92" t="s">
         <v>277</v>
@@ -7153,7 +7174,7 @@
         <v>276</v>
       </c>
       <c r="Q92" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
@@ -7188,7 +7209,7 @@
         <v>338</v>
       </c>
       <c r="N93" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O93" t="s">
         <v>277</v>
@@ -7197,7 +7218,7 @@
         <v>276</v>
       </c>
       <c r="Q93" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
@@ -7232,7 +7253,7 @@
         <v>340</v>
       </c>
       <c r="N94" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O94" t="s">
         <v>277</v>
@@ -7241,7 +7262,7 @@
         <v>276</v>
       </c>
       <c r="Q94" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
@@ -7276,7 +7297,7 @@
         <v>342</v>
       </c>
       <c r="N95" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O95" t="s">
         <v>277</v>
@@ -7285,7 +7306,7 @@
         <v>276</v>
       </c>
       <c r="Q95" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
@@ -7320,7 +7341,7 @@
         <v>344</v>
       </c>
       <c r="N96" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O96" t="s">
         <v>277</v>
@@ -7329,7 +7350,7 @@
         <v>276</v>
       </c>
       <c r="Q96" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
@@ -7364,7 +7385,7 @@
         <v>346</v>
       </c>
       <c r="N97" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O97" t="s">
         <v>277</v>
@@ -7373,7 +7394,7 @@
         <v>276</v>
       </c>
       <c r="Q97" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
@@ -7408,7 +7429,7 @@
         <v>348</v>
       </c>
       <c r="N98" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O98" t="s">
         <v>277</v>
@@ -7417,7 +7438,7 @@
         <v>276</v>
       </c>
       <c r="Q98" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
@@ -7452,7 +7473,7 @@
         <v>350</v>
       </c>
       <c r="N99" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O99" t="s">
         <v>277</v>
@@ -7461,7 +7482,7 @@
         <v>276</v>
       </c>
       <c r="Q99" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
@@ -7496,7 +7517,7 @@
         <v>352</v>
       </c>
       <c r="N100" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O100" t="s">
         <v>277</v>
@@ -7505,7 +7526,7 @@
         <v>276</v>
       </c>
       <c r="Q100" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
@@ -7540,7 +7561,7 @@
         <v>354</v>
       </c>
       <c r="N101" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O101" t="s">
         <v>277</v>
@@ -7549,7 +7570,7 @@
         <v>276</v>
       </c>
       <c r="Q101" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
@@ -7584,7 +7605,7 @@
         <v>356</v>
       </c>
       <c r="N102" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O102" t="s">
         <v>277</v>
@@ -7593,7 +7614,7 @@
         <v>276</v>
       </c>
       <c r="Q102" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
@@ -7628,7 +7649,7 @@
         <v>357</v>
       </c>
       <c r="N103" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O103" t="s">
         <v>277</v>
@@ -7637,7 +7658,7 @@
         <v>276</v>
       </c>
       <c r="Q103" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
@@ -7672,7 +7693,7 @@
         <v>358</v>
       </c>
       <c r="N104" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O104" t="s">
         <v>277</v>
@@ -7681,7 +7702,7 @@
         <v>276</v>
       </c>
       <c r="Q104" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
@@ -7716,7 +7737,7 @@
         <v>359</v>
       </c>
       <c r="N105" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O105" t="s">
         <v>277</v>
@@ -7725,7 +7746,7 @@
         <v>276</v>
       </c>
       <c r="Q105" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
@@ -7760,7 +7781,7 @@
         <v>361</v>
       </c>
       <c r="N106" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O106" t="s">
         <v>277</v>
@@ -7769,7 +7790,7 @@
         <v>276</v>
       </c>
       <c r="Q106" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
@@ -7804,7 +7825,7 @@
         <v>363</v>
       </c>
       <c r="N107" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O107" t="s">
         <v>277</v>
@@ -7813,7 +7834,7 @@
         <v>276</v>
       </c>
       <c r="Q107" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
@@ -7848,7 +7869,7 @@
         <v>365</v>
       </c>
       <c r="N108" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O108" t="s">
         <v>277</v>
@@ -7857,7 +7878,7 @@
         <v>276</v>
       </c>
       <c r="Q108" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
@@ -7892,7 +7913,7 @@
         <v>367</v>
       </c>
       <c r="N109" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O109" t="s">
         <v>277</v>
@@ -7901,7 +7922,7 @@
         <v>276</v>
       </c>
       <c r="Q109" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
@@ -7936,7 +7957,7 @@
         <v>369</v>
       </c>
       <c r="N110" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O110" t="s">
         <v>277</v>
@@ -7945,7 +7966,7 @@
         <v>276</v>
       </c>
       <c r="Q110" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
@@ -7980,7 +8001,7 @@
         <v>371</v>
       </c>
       <c r="N111" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O111" t="s">
         <v>277</v>
@@ -7989,7 +8010,7 @@
         <v>276</v>
       </c>
       <c r="Q111" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
@@ -8024,7 +8045,7 @@
         <v>373</v>
       </c>
       <c r="N112" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O112" t="s">
         <v>277</v>
@@ -8033,7 +8054,7 @@
         <v>276</v>
       </c>
       <c r="Q112" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
@@ -8068,7 +8089,7 @@
         <v>375</v>
       </c>
       <c r="N113" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O113" t="s">
         <v>277</v>
@@ -8077,7 +8098,7 @@
         <v>276</v>
       </c>
       <c r="Q113" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
@@ -8112,7 +8133,7 @@
         <v>377</v>
       </c>
       <c r="N114" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O114" t="s">
         <v>277</v>
@@ -8121,7 +8142,7 @@
         <v>276</v>
       </c>
       <c r="Q114" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
@@ -8156,7 +8177,7 @@
         <v>379</v>
       </c>
       <c r="N115" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O115" t="s">
         <v>277</v>
@@ -8165,7 +8186,7 @@
         <v>276</v>
       </c>
       <c r="Q115" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.25">
@@ -8203,7 +8224,7 @@
         <v>389</v>
       </c>
       <c r="N116" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O116" t="s">
         <v>281</v>
@@ -8212,7 +8233,7 @@
         <v>280</v>
       </c>
       <c r="Q116" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
@@ -8250,7 +8271,7 @@
         <v>391</v>
       </c>
       <c r="N117" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O117" t="s">
         <v>281</v>
@@ -8259,7 +8280,7 @@
         <v>280</v>
       </c>
       <c r="Q117" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
@@ -8297,7 +8318,7 @@
         <v>393</v>
       </c>
       <c r="N118" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O118" t="s">
         <v>281</v>
@@ -8306,7 +8327,7 @@
         <v>280</v>
       </c>
       <c r="Q118" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
@@ -8344,7 +8365,7 @@
         <v>389</v>
       </c>
       <c r="N119" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O119" t="s">
         <v>281</v>
@@ -8353,7 +8374,7 @@
         <v>280</v>
       </c>
       <c r="Q119" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.25">
@@ -8391,7 +8412,7 @@
         <v>391</v>
       </c>
       <c r="N120" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O120" t="s">
         <v>281</v>
@@ -8400,7 +8421,7 @@
         <v>280</v>
       </c>
       <c r="Q120" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
@@ -8438,7 +8459,7 @@
         <v>393</v>
       </c>
       <c r="N121" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O121" t="s">
         <v>281</v>
@@ -8447,7 +8468,7 @@
         <v>280</v>
       </c>
       <c r="Q121" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
@@ -8485,7 +8506,7 @@
         <v>396</v>
       </c>
       <c r="N122" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O122" t="s">
         <v>281</v>
@@ -8494,7 +8515,7 @@
         <v>280</v>
       </c>
       <c r="Q122" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
@@ -8532,7 +8553,7 @@
         <v>399</v>
       </c>
       <c r="N123" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O123" t="s">
         <v>281</v>
@@ -8541,7 +8562,7 @@
         <v>280</v>
       </c>
       <c r="Q123" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
@@ -8579,7 +8600,7 @@
         <v>402</v>
       </c>
       <c r="N124" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O124" t="s">
         <v>281</v>
@@ -8588,7 +8609,7 @@
         <v>280</v>
       </c>
       <c r="Q124" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
@@ -8626,7 +8647,7 @@
         <v>396</v>
       </c>
       <c r="N125" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O125" t="s">
         <v>281</v>
@@ -8635,7 +8656,7 @@
         <v>280</v>
       </c>
       <c r="Q125" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.25">
@@ -8673,7 +8694,7 @@
         <v>399</v>
       </c>
       <c r="N126" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O126" t="s">
         <v>281</v>
@@ -8682,7 +8703,7 @@
         <v>280</v>
       </c>
       <c r="Q126" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.25">
@@ -8720,7 +8741,7 @@
         <v>402</v>
       </c>
       <c r="N127" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O127" t="s">
         <v>281</v>
@@ -8729,7 +8750,7 @@
         <v>280</v>
       </c>
       <c r="Q127" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.25">
@@ -8761,13 +8782,13 @@
         <v>433</v>
       </c>
       <c r="N128" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O128" t="s">
         <v>281</v>
       </c>
       <c r="Q128" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
@@ -8799,13 +8820,13 @@
         <v>434</v>
       </c>
       <c r="N129" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O129" t="s">
         <v>280</v>
       </c>
       <c r="Q129" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.25">
@@ -8840,7 +8861,7 @@
         <v>435</v>
       </c>
       <c r="N130" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O130" t="s">
         <v>281</v>
@@ -8849,7 +8870,7 @@
         <v>280</v>
       </c>
       <c r="Q130" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
@@ -8881,13 +8902,13 @@
         <v>437</v>
       </c>
       <c r="N131" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O131" t="s">
         <v>281</v>
       </c>
       <c r="Q131" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
@@ -8919,13 +8940,13 @@
         <v>439</v>
       </c>
       <c r="N132" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O132" t="s">
         <v>280</v>
       </c>
       <c r="Q132" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
@@ -8960,7 +8981,7 @@
         <v>441</v>
       </c>
       <c r="N133" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O133" t="s">
         <v>281</v>
@@ -8969,7 +8990,7 @@
         <v>280</v>
       </c>
       <c r="Q133" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.25">
@@ -9001,13 +9022,13 @@
         <v>443</v>
       </c>
       <c r="N134" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O134" t="s">
         <v>281</v>
       </c>
       <c r="Q134" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.25">
@@ -9039,13 +9060,13 @@
         <v>445</v>
       </c>
       <c r="N135" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O135" t="s">
         <v>280</v>
       </c>
       <c r="Q135" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
@@ -9080,7 +9101,7 @@
         <v>447</v>
       </c>
       <c r="N136" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O136" t="s">
         <v>281</v>
@@ -9089,7 +9110,7 @@
         <v>280</v>
       </c>
       <c r="Q136" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.25">
@@ -9121,13 +9142,13 @@
         <v>449</v>
       </c>
       <c r="N137" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O137" t="s">
         <v>281</v>
       </c>
       <c r="Q137" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
@@ -9159,13 +9180,13 @@
         <v>451</v>
       </c>
       <c r="N138" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O138" t="s">
         <v>280</v>
       </c>
       <c r="Q138" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
@@ -9200,7 +9221,7 @@
         <v>453</v>
       </c>
       <c r="N139" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O139" t="s">
         <v>281</v>
@@ -9209,7 +9230,7 @@
         <v>280</v>
       </c>
       <c r="Q139" t="s">
-        <v>321</v>
+        <v>506</v>
       </c>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
@@ -9241,7 +9262,7 @@
         <v>459</v>
       </c>
       <c r="N140" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O140" t="s">
         <v>281</v>
@@ -9282,7 +9303,7 @@
         <v>459</v>
       </c>
       <c r="N141" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O141" t="s">
         <v>280</v>
@@ -9326,7 +9347,7 @@
         <v>459</v>
       </c>
       <c r="N142" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O142" t="s">
         <v>281</v>
@@ -9370,7 +9391,7 @@
         <v>461</v>
       </c>
       <c r="N143" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O143" t="s">
         <v>281</v>
@@ -9411,7 +9432,7 @@
         <v>461</v>
       </c>
       <c r="N144" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O144" t="s">
         <v>280</v>
@@ -9455,7 +9476,7 @@
         <v>461</v>
       </c>
       <c r="N145" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O145" t="s">
         <v>281</v>
@@ -9499,7 +9520,7 @@
         <v>464</v>
       </c>
       <c r="N146" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O146" t="s">
         <v>281</v>
@@ -9540,7 +9561,7 @@
         <v>464</v>
       </c>
       <c r="N147" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O147" t="s">
         <v>280</v>
@@ -9584,7 +9605,7 @@
         <v>464</v>
       </c>
       <c r="N148" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O148" t="s">
         <v>281</v>
@@ -9628,7 +9649,7 @@
         <v>465</v>
       </c>
       <c r="N149" s="18" t="s">
-        <v>328</v>
+        <v>503</v>
       </c>
       <c r="O149" t="s">
         <v>281</v>
@@ -9669,7 +9690,7 @@
         <v>465</v>
       </c>
       <c r="N150" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O150" t="s">
         <v>280</v>
@@ -9713,7 +9734,7 @@
         <v>465</v>
       </c>
       <c r="N151" s="18" t="s">
-        <v>328</v>
+        <v>502</v>
       </c>
       <c r="O151" t="s">
         <v>281</v>
@@ -13390,10 +13411,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13806,6 +13827,30 @@
       </c>
       <c r="B46" t="s">
         <v>483</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>501</v>
+      </c>
+      <c r="B47" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>502</v>
+      </c>
+      <c r="B48" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>503</v>
+      </c>
+      <c r="B49" t="s">
+        <v>505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
forgot inducers for one date
</commit_message>
<xml_diff>
--- a/input/datasets.xlsx
+++ b/input/datasets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="alldata" sheetId="1" r:id="rId1"/>
@@ -2700,9 +2700,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U180" sqref="U180"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13266,10 +13266,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13278,7 +13278,7 @@
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
@@ -13304,7 +13304,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -13332,7 +13332,7 @@
         <v>150.14166666666671</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
@@ -13357,7 +13357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>54</v>
       </c>
@@ -13385,7 +13385,7 @@
         <v>1.9994000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
@@ -13413,7 +13413,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>57</v>
       </c>
@@ -13441,7 +13441,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>46</v>
       </c>
@@ -13466,7 +13466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>58</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>59</v>
       </c>
@@ -13519,7 +13519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>60</v>
       </c>
@@ -13544,7 +13544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
@@ -13569,7 +13569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>62</v>
       </c>
@@ -13594,12 +13594,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>275</v>
       </c>
@@ -13613,37 +13613,40 @@
         <v>181113</v>
       </c>
       <c r="E14">
+        <v>181203</v>
+      </c>
+      <c r="F14">
         <v>190118</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>190207</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>190228</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>190308</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>190417</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>191011</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>191114</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>200131</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>201125</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>201212</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -13658,37 +13661,40 @@
         <v>90</v>
       </c>
       <c r="E15">
+        <v>90</v>
+      </c>
+      <c r="F15">
         <v>300</v>
-      </c>
-      <c r="F15">
-        <v>15</v>
       </c>
       <c r="G15">
         <v>15</v>
       </c>
       <c r="H15">
+        <v>15</v>
+      </c>
+      <c r="I15">
         <v>150</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>30</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>300</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>286</v>
-      </c>
-      <c r="L15">
-        <v>300</v>
       </c>
       <c r="M15">
         <v>300</v>
       </c>
       <c r="N15">
+        <v>300</v>
+      </c>
+      <c r="O15">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -13702,17 +13708,20 @@
         <f>C2</f>
         <v>300</v>
       </c>
-      <c r="F16">
+      <c r="E16">
+        <v>150</v>
+      </c>
+      <c r="G16">
         <v>45</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>300</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -13722,36 +13731,36 @@
       <c r="C17">
         <v>200</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>120</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>112</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>300</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>331</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>300</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -13763,16 +13772,16 @@
         <v>0.2</v>
       </c>
       <c r="E20">
+        <v>0.2</v>
+      </c>
+      <c r="F20">
         <v>2</v>
-      </c>
-      <c r="F20">
-        <v>0.6</v>
       </c>
       <c r="G20">
         <v>0.6</v>
       </c>
       <c r="H20">
-        <v>2</v>
+        <v>0.6</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -13792,8 +13801,11 @@
       <c r="N20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -13834,8 +13846,11 @@
       <c r="N21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -13843,7 +13858,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -13851,7 +13866,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -13862,23 +13877,23 @@
         <f>0.3*C6</f>
         <v>30</v>
       </c>
-      <c r="F24">
+      <c r="E24">
+        <v>30</v>
+      </c>
+      <c r="G24">
         <v>5</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>15</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>100</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>10</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>5</v>
-      </c>
-      <c r="K24">
-        <v>100</v>
       </c>
       <c r="L24">
         <v>100</v>
@@ -13887,10 +13902,13 @@
         <v>100</v>
       </c>
       <c r="N24">
+        <v>100</v>
+      </c>
+      <c r="O24">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -13901,58 +13919,61 @@
         <f>C6</f>
         <v>100</v>
       </c>
-      <c r="F25">
+      <c r="E25">
+        <v>50</v>
+      </c>
+      <c r="G25">
         <v>15</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>100</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>30</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>20</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>110</v>
       </c>
       <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>40</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>50</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>111</v>
       </c>
       <c r="B27" t="s">
         <v>56</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>100</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>330</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated seq id and added datasets
</commit_message>
<xml_diff>
--- a/input/datasets.xlsx
+++ b/input/datasets.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3507" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3775" uniqueCount="559">
   <si>
     <t>date_sequenced</t>
   </si>
@@ -1621,6 +1621,87 @@
   </si>
   <si>
     <t>24.17,[sal,atc,cin]</t>
+  </si>
+  <si>
+    <t>210429</t>
+  </si>
+  <si>
+    <t>24,[sal]</t>
+  </si>
+  <si>
+    <t>24,[sal,atc]</t>
+  </si>
+  <si>
+    <t>24,[sal,atc,cin]</t>
+  </si>
+  <si>
+    <t>24,[sal,atc,ara]</t>
+  </si>
+  <si>
+    <t>RBK004</t>
+  </si>
+  <si>
+    <t>210507</t>
+  </si>
+  <si>
+    <t>10,[]</t>
+  </si>
+  <si>
+    <t>210603</t>
+  </si>
+  <si>
+    <t>ara1</t>
+  </si>
+  <si>
+    <t>ara2</t>
+  </si>
+  <si>
+    <t>10,[atc]</t>
+  </si>
+  <si>
+    <t>25,[atc,sal]</t>
+  </si>
+  <si>
+    <t>10,[atc,ara2]</t>
+  </si>
+  <si>
+    <t>25,[atc,ara2,sal]</t>
+  </si>
+  <si>
+    <t>10,[atc,ara1]</t>
+  </si>
+  <si>
+    <t>25,[atc,ara1,sal]</t>
+  </si>
+  <si>
+    <t>10,[arc,ara]</t>
+  </si>
+  <si>
+    <t>25,[arc,ara,sal]</t>
+  </si>
+  <si>
+    <t>10,[atc,cin2]</t>
+  </si>
+  <si>
+    <t>25,[atc,cin2,sal]</t>
+  </si>
+  <si>
+    <t>10,[atc,cin1]</t>
+  </si>
+  <si>
+    <t>25,[atc,cin1,sal]</t>
+  </si>
+  <si>
+    <t>10,[atc,cin]</t>
+  </si>
+  <si>
+    <t>25,[atc,cin,sal]</t>
+  </si>
+  <si>
+    <t>25,[atc,ara2,sal1]</t>
+  </si>
+  <si>
+    <t>25,[atc,cin2,sal1]</t>
   </si>
 </sst>
 </file>
@@ -2770,17 +2851,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S207"/>
+  <dimension ref="A1:S228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H194" sqref="H194"/>
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I188" sqref="I188:J188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="17"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12906,6 +12990,900 @@
         <v>318</v>
       </c>
       <c r="S207" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A208" s="17" t="s">
+        <v>532</v>
+      </c>
+      <c r="B208" t="s">
+        <v>19</v>
+      </c>
+      <c r="D208" t="s">
+        <v>482</v>
+      </c>
+      <c r="E208" t="s">
+        <v>452</v>
+      </c>
+      <c r="F208" t="s">
+        <v>453</v>
+      </c>
+      <c r="I208" t="s">
+        <v>92</v>
+      </c>
+      <c r="M208" s="1">
+        <v>44301</v>
+      </c>
+      <c r="N208" t="s">
+        <v>483</v>
+      </c>
+      <c r="O208" t="s">
+        <v>278</v>
+      </c>
+      <c r="P208" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q208" t="s">
+        <v>318</v>
+      </c>
+      <c r="R208" t="s">
+        <v>537</v>
+      </c>
+      <c r="S208" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A209" s="17" t="s">
+        <v>532</v>
+      </c>
+      <c r="B209" t="s">
+        <v>20</v>
+      </c>
+      <c r="D209" t="s">
+        <v>482</v>
+      </c>
+      <c r="E209" t="s">
+        <v>452</v>
+      </c>
+      <c r="F209" t="s">
+        <v>453</v>
+      </c>
+      <c r="I209" t="s">
+        <v>533</v>
+      </c>
+      <c r="M209" s="1">
+        <v>44301</v>
+      </c>
+      <c r="N209" t="s">
+        <v>483</v>
+      </c>
+      <c r="O209" t="s">
+        <v>278</v>
+      </c>
+      <c r="P209" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q209" t="s">
+        <v>318</v>
+      </c>
+      <c r="R209" t="s">
+        <v>537</v>
+      </c>
+      <c r="S209" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A210" s="17" t="s">
+        <v>532</v>
+      </c>
+      <c r="B210" t="s">
+        <v>21</v>
+      </c>
+      <c r="D210" t="s">
+        <v>482</v>
+      </c>
+      <c r="E210" t="s">
+        <v>452</v>
+      </c>
+      <c r="F210" t="s">
+        <v>453</v>
+      </c>
+      <c r="I210" t="s">
+        <v>534</v>
+      </c>
+      <c r="M210" s="1">
+        <v>44301</v>
+      </c>
+      <c r="N210" t="s">
+        <v>483</v>
+      </c>
+      <c r="O210" t="s">
+        <v>278</v>
+      </c>
+      <c r="P210" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q210" t="s">
+        <v>318</v>
+      </c>
+      <c r="R210" t="s">
+        <v>537</v>
+      </c>
+      <c r="S210" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A211" s="17" t="s">
+        <v>532</v>
+      </c>
+      <c r="B211" t="s">
+        <v>22</v>
+      </c>
+      <c r="D211" t="s">
+        <v>482</v>
+      </c>
+      <c r="E211" t="s">
+        <v>452</v>
+      </c>
+      <c r="F211" t="s">
+        <v>453</v>
+      </c>
+      <c r="I211" t="s">
+        <v>535</v>
+      </c>
+      <c r="M211" s="1">
+        <v>44301</v>
+      </c>
+      <c r="N211" t="s">
+        <v>483</v>
+      </c>
+      <c r="O211" t="s">
+        <v>278</v>
+      </c>
+      <c r="P211" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q211" t="s">
+        <v>318</v>
+      </c>
+      <c r="R211" t="s">
+        <v>537</v>
+      </c>
+      <c r="S211" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A212" s="17" t="s">
+        <v>532</v>
+      </c>
+      <c r="B212" t="s">
+        <v>23</v>
+      </c>
+      <c r="D212" t="s">
+        <v>482</v>
+      </c>
+      <c r="E212" t="s">
+        <v>452</v>
+      </c>
+      <c r="F212" t="s">
+        <v>453</v>
+      </c>
+      <c r="I212" t="s">
+        <v>536</v>
+      </c>
+      <c r="M212" s="1">
+        <v>44301</v>
+      </c>
+      <c r="N212" t="s">
+        <v>483</v>
+      </c>
+      <c r="O212" t="s">
+        <v>278</v>
+      </c>
+      <c r="P212" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q212" t="s">
+        <v>318</v>
+      </c>
+      <c r="R212" t="s">
+        <v>537</v>
+      </c>
+      <c r="S212" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A213" s="17" t="s">
+        <v>538</v>
+      </c>
+      <c r="B213" t="s">
+        <v>66</v>
+      </c>
+      <c r="D213" t="s">
+        <v>482</v>
+      </c>
+      <c r="E213" t="s">
+        <v>452</v>
+      </c>
+      <c r="F213" t="s">
+        <v>453</v>
+      </c>
+      <c r="I213" t="s">
+        <v>92</v>
+      </c>
+      <c r="M213" s="1">
+        <v>44319</v>
+      </c>
+      <c r="N213" t="s">
+        <v>483</v>
+      </c>
+      <c r="O213" t="s">
+        <v>278</v>
+      </c>
+      <c r="P213" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q213" t="s">
+        <v>318</v>
+      </c>
+      <c r="R213" t="s">
+        <v>537</v>
+      </c>
+      <c r="S213" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A214" s="17" t="s">
+        <v>538</v>
+      </c>
+      <c r="B214" t="s">
+        <v>24</v>
+      </c>
+      <c r="D214" t="s">
+        <v>482</v>
+      </c>
+      <c r="E214" t="s">
+        <v>452</v>
+      </c>
+      <c r="F214" t="s">
+        <v>453</v>
+      </c>
+      <c r="I214" t="s">
+        <v>533</v>
+      </c>
+      <c r="M214" s="1">
+        <v>44319</v>
+      </c>
+      <c r="N214" t="s">
+        <v>483</v>
+      </c>
+      <c r="O214" t="s">
+        <v>278</v>
+      </c>
+      <c r="P214" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q214" t="s">
+        <v>318</v>
+      </c>
+      <c r="R214" t="s">
+        <v>537</v>
+      </c>
+      <c r="S214" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A215" s="17" t="s">
+        <v>538</v>
+      </c>
+      <c r="B215" t="s">
+        <v>25</v>
+      </c>
+      <c r="D215" t="s">
+        <v>482</v>
+      </c>
+      <c r="E215" t="s">
+        <v>452</v>
+      </c>
+      <c r="F215" t="s">
+        <v>453</v>
+      </c>
+      <c r="I215" t="s">
+        <v>534</v>
+      </c>
+      <c r="M215" s="1">
+        <v>44319</v>
+      </c>
+      <c r="N215" t="s">
+        <v>483</v>
+      </c>
+      <c r="O215" t="s">
+        <v>278</v>
+      </c>
+      <c r="P215" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q215" t="s">
+        <v>318</v>
+      </c>
+      <c r="R215" t="s">
+        <v>537</v>
+      </c>
+      <c r="S215" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A216" s="17" t="s">
+        <v>538</v>
+      </c>
+      <c r="B216" t="s">
+        <v>26</v>
+      </c>
+      <c r="D216" t="s">
+        <v>482</v>
+      </c>
+      <c r="E216" t="s">
+        <v>452</v>
+      </c>
+      <c r="F216" t="s">
+        <v>453</v>
+      </c>
+      <c r="I216" t="s">
+        <v>535</v>
+      </c>
+      <c r="M216" s="1">
+        <v>44319</v>
+      </c>
+      <c r="N216" t="s">
+        <v>483</v>
+      </c>
+      <c r="O216" t="s">
+        <v>278</v>
+      </c>
+      <c r="P216" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q216" t="s">
+        <v>318</v>
+      </c>
+      <c r="R216" t="s">
+        <v>537</v>
+      </c>
+      <c r="S216" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A217" s="17" t="s">
+        <v>538</v>
+      </c>
+      <c r="B217" t="s">
+        <v>27</v>
+      </c>
+      <c r="D217" t="s">
+        <v>482</v>
+      </c>
+      <c r="E217" t="s">
+        <v>452</v>
+      </c>
+      <c r="F217" t="s">
+        <v>453</v>
+      </c>
+      <c r="I217" t="s">
+        <v>536</v>
+      </c>
+      <c r="M217" s="1">
+        <v>44319</v>
+      </c>
+      <c r="N217" t="s">
+        <v>483</v>
+      </c>
+      <c r="O217" t="s">
+        <v>278</v>
+      </c>
+      <c r="P217" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q217" t="s">
+        <v>318</v>
+      </c>
+      <c r="R217" t="s">
+        <v>537</v>
+      </c>
+      <c r="S217" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A218" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B218" t="s">
+        <v>20</v>
+      </c>
+      <c r="D218" t="s">
+        <v>482</v>
+      </c>
+      <c r="E218" t="s">
+        <v>452</v>
+      </c>
+      <c r="F218" t="s">
+        <v>453</v>
+      </c>
+      <c r="I218" t="s">
+        <v>539</v>
+      </c>
+      <c r="J218" t="s">
+        <v>488</v>
+      </c>
+      <c r="M218" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N218" t="s">
+        <v>483</v>
+      </c>
+      <c r="O218" t="s">
+        <v>278</v>
+      </c>
+      <c r="P218" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q218" t="s">
+        <v>318</v>
+      </c>
+      <c r="R218" t="s">
+        <v>537</v>
+      </c>
+      <c r="S218" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A219" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B219" t="s">
+        <v>21</v>
+      </c>
+      <c r="D219" t="s">
+        <v>482</v>
+      </c>
+      <c r="E219" t="s">
+        <v>452</v>
+      </c>
+      <c r="F219" t="s">
+        <v>453</v>
+      </c>
+      <c r="I219" t="s">
+        <v>543</v>
+      </c>
+      <c r="J219" t="s">
+        <v>544</v>
+      </c>
+      <c r="M219" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N219" t="s">
+        <v>483</v>
+      </c>
+      <c r="O219" t="s">
+        <v>278</v>
+      </c>
+      <c r="P219" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q219" t="s">
+        <v>318</v>
+      </c>
+      <c r="R219" t="s">
+        <v>537</v>
+      </c>
+      <c r="S219" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A220" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B220" t="s">
+        <v>22</v>
+      </c>
+      <c r="D220" t="s">
+        <v>482</v>
+      </c>
+      <c r="E220" t="s">
+        <v>452</v>
+      </c>
+      <c r="F220" t="s">
+        <v>453</v>
+      </c>
+      <c r="I220" t="s">
+        <v>545</v>
+      </c>
+      <c r="J220" t="s">
+        <v>546</v>
+      </c>
+      <c r="M220" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N220" t="s">
+        <v>483</v>
+      </c>
+      <c r="O220" t="s">
+        <v>278</v>
+      </c>
+      <c r="P220" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q220" t="s">
+        <v>318</v>
+      </c>
+      <c r="R220" t="s">
+        <v>537</v>
+      </c>
+      <c r="S220" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A221" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B221" t="s">
+        <v>23</v>
+      </c>
+      <c r="D221" t="s">
+        <v>482</v>
+      </c>
+      <c r="E221" t="s">
+        <v>452</v>
+      </c>
+      <c r="F221" t="s">
+        <v>453</v>
+      </c>
+      <c r="I221" t="s">
+        <v>547</v>
+      </c>
+      <c r="J221" t="s">
+        <v>548</v>
+      </c>
+      <c r="M221" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N221" t="s">
+        <v>483</v>
+      </c>
+      <c r="O221" t="s">
+        <v>278</v>
+      </c>
+      <c r="P221" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q221" t="s">
+        <v>318</v>
+      </c>
+      <c r="R221" t="s">
+        <v>537</v>
+      </c>
+      <c r="S221" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A222" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B222" t="s">
+        <v>66</v>
+      </c>
+      <c r="D222" t="s">
+        <v>482</v>
+      </c>
+      <c r="E222" t="s">
+        <v>452</v>
+      </c>
+      <c r="F222" t="s">
+        <v>453</v>
+      </c>
+      <c r="I222" t="s">
+        <v>549</v>
+      </c>
+      <c r="J222" t="s">
+        <v>550</v>
+      </c>
+      <c r="M222" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N222" t="s">
+        <v>483</v>
+      </c>
+      <c r="O222" t="s">
+        <v>278</v>
+      </c>
+      <c r="P222" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q222" t="s">
+        <v>318</v>
+      </c>
+      <c r="R222" t="s">
+        <v>537</v>
+      </c>
+      <c r="S222" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A223" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B223" t="s">
+        <v>24</v>
+      </c>
+      <c r="D223" t="s">
+        <v>482</v>
+      </c>
+      <c r="E223" t="s">
+        <v>452</v>
+      </c>
+      <c r="F223" t="s">
+        <v>453</v>
+      </c>
+      <c r="I223" t="s">
+        <v>551</v>
+      </c>
+      <c r="J223" t="s">
+        <v>552</v>
+      </c>
+      <c r="M223" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N223" t="s">
+        <v>483</v>
+      </c>
+      <c r="O223" t="s">
+        <v>278</v>
+      </c>
+      <c r="P223" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q223" t="s">
+        <v>318</v>
+      </c>
+      <c r="R223" t="s">
+        <v>537</v>
+      </c>
+      <c r="S223" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A224" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B224" t="s">
+        <v>25</v>
+      </c>
+      <c r="D224" t="s">
+        <v>482</v>
+      </c>
+      <c r="E224" t="s">
+        <v>452</v>
+      </c>
+      <c r="F224" t="s">
+        <v>453</v>
+      </c>
+      <c r="I224" t="s">
+        <v>553</v>
+      </c>
+      <c r="J224" t="s">
+        <v>554</v>
+      </c>
+      <c r="M224" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N224" t="s">
+        <v>483</v>
+      </c>
+      <c r="O224" t="s">
+        <v>278</v>
+      </c>
+      <c r="P224" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q224" t="s">
+        <v>318</v>
+      </c>
+      <c r="R224" t="s">
+        <v>537</v>
+      </c>
+      <c r="S224" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="225" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A225" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B225" t="s">
+        <v>26</v>
+      </c>
+      <c r="D225" t="s">
+        <v>482</v>
+      </c>
+      <c r="E225" t="s">
+        <v>452</v>
+      </c>
+      <c r="F225" t="s">
+        <v>453</v>
+      </c>
+      <c r="I225" t="s">
+        <v>555</v>
+      </c>
+      <c r="J225" t="s">
+        <v>556</v>
+      </c>
+      <c r="M225" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N225" t="s">
+        <v>483</v>
+      </c>
+      <c r="O225" t="s">
+        <v>278</v>
+      </c>
+      <c r="P225" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q225" t="s">
+        <v>318</v>
+      </c>
+      <c r="R225" t="s">
+        <v>537</v>
+      </c>
+      <c r="S225" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="226" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A226" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B226" t="s">
+        <v>27</v>
+      </c>
+      <c r="D226" t="s">
+        <v>482</v>
+      </c>
+      <c r="E226" t="s">
+        <v>452</v>
+      </c>
+      <c r="F226" t="s">
+        <v>453</v>
+      </c>
+      <c r="I226" t="s">
+        <v>545</v>
+      </c>
+      <c r="J226" t="s">
+        <v>557</v>
+      </c>
+      <c r="M226" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N226" t="s">
+        <v>483</v>
+      </c>
+      <c r="O226" t="s">
+        <v>278</v>
+      </c>
+      <c r="P226" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q226" t="s">
+        <v>318</v>
+      </c>
+      <c r="R226" t="s">
+        <v>537</v>
+      </c>
+      <c r="S226" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="227" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A227" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B227" t="s">
+        <v>28</v>
+      </c>
+      <c r="D227" t="s">
+        <v>482</v>
+      </c>
+      <c r="E227" t="s">
+        <v>452</v>
+      </c>
+      <c r="F227" t="s">
+        <v>453</v>
+      </c>
+      <c r="I227" t="s">
+        <v>551</v>
+      </c>
+      <c r="J227" t="s">
+        <v>558</v>
+      </c>
+      <c r="M227" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N227" t="s">
+        <v>483</v>
+      </c>
+      <c r="O227" t="s">
+        <v>278</v>
+      </c>
+      <c r="P227" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q227" t="s">
+        <v>318</v>
+      </c>
+      <c r="R227" t="s">
+        <v>537</v>
+      </c>
+      <c r="S227" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="228" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A228" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B228" t="s">
+        <v>70</v>
+      </c>
+      <c r="D228" t="s">
+        <v>482</v>
+      </c>
+      <c r="E228" t="s">
+        <v>452</v>
+      </c>
+      <c r="F228" t="s">
+        <v>453</v>
+      </c>
+      <c r="I228" t="s">
+        <v>539</v>
+      </c>
+      <c r="J228" t="s">
+        <v>78</v>
+      </c>
+      <c r="M228" s="1">
+        <v>44345</v>
+      </c>
+      <c r="N228" t="s">
+        <v>483</v>
+      </c>
+      <c r="O228" t="s">
+        <v>278</v>
+      </c>
+      <c r="P228" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q228" t="s">
+        <v>318</v>
+      </c>
+      <c r="R228" t="s">
+        <v>537</v>
+      </c>
+      <c r="S228" t="s">
         <v>57</v>
       </c>
     </row>
@@ -14466,10 +15444,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14478,7 +15456,7 @@
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
@@ -14504,7 +15482,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -14532,7 +15510,7 @@
         <v>150.14166666666671</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
@@ -14557,7 +15535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>54</v>
       </c>
@@ -14585,7 +15563,7 @@
         <v>1.9994000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
@@ -14613,7 +15591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>57</v>
       </c>
@@ -14641,7 +15619,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>46</v>
       </c>
@@ -14666,7 +15644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>58</v>
       </c>
@@ -14694,7 +15672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>59</v>
       </c>
@@ -14719,7 +15697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>60</v>
       </c>
@@ -14744,7 +15722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
@@ -14769,7 +15747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>62</v>
       </c>
@@ -14794,12 +15772,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>272</v>
       </c>
@@ -14851,8 +15829,17 @@
       <c r="Q14">
         <v>210223</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="17" t="s">
+        <v>532</v>
+      </c>
+      <c r="S14">
+        <v>210507</v>
+      </c>
+      <c r="T14">
+        <v>210603</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -14905,8 +15892,20 @@
       <c r="Q15">
         <v>300</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <f>4300000*34.88/500000</f>
+        <v>299.96800000000002</v>
+      </c>
+      <c r="S15">
+        <f>430000*6.977*40/(100*4000)</f>
+        <v>300.01100000000002</v>
+      </c>
+      <c r="T15">
+        <f>430000*1.05*2/15/200</f>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -14936,7 +15935,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -14956,7 +15955,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -14973,7 +15972,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>328</v>
       </c>
@@ -14981,7 +15980,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -15031,8 +16030,20 @@
       <c r="Q20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <f>1300*769.2/500000</f>
+        <v>1.9999200000000001</v>
+      </c>
+      <c r="S20">
+        <f>1300*15.38*40/(100*4000)</f>
+        <v>1.9994000000000001</v>
+      </c>
+      <c r="T20">
+        <f>1300*0.23*2/15/200</f>
+        <v>0.19933333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -15082,24 +16093,44 @@
       <c r="Q21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <f>50000*50/500000</f>
+        <v>5</v>
+      </c>
+      <c r="S21">
+        <f>50000*1*40/(100*4000)</f>
+        <v>5</v>
+      </c>
+      <c r="T21">
+        <f>2500*0.3*2/15/200</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T22">
+        <f>2500*1.5*2/15/200</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
       <c r="B23" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T23">
+        <f>2500*3*2/15/200</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -15146,8 +16177,20 @@
       <c r="Q24">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <f>100*500000/500000</f>
+        <v>100</v>
+      </c>
+      <c r="S24">
+        <f>500000*2*40/(100*4000)</f>
+        <v>100</v>
+      </c>
+      <c r="T24">
+        <f>100000*8*2/80/200</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -15179,8 +16222,12 @@
       <c r="P25">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T25">
+        <f>100000*2.4*2/80/200</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -15200,7 +16247,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>111</v>
       </c>
@@ -15217,12 +16264,36 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>327</v>
       </c>
       <c r="K28">
         <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>541</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="T29">
+        <f>1300*1.15*2/15/200</f>
+        <v>0.99666666666666659</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>542</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="T30">
+        <f>1300*2.31*2/15/200</f>
+        <v>2.0019999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>